<commit_message>
Update: Them ket qua test sai so giua 2 RPi
</commit_message>
<xml_diff>
--- a/Documents/RPi NTP Time Server Statrum-2/Test/TestLog.xlsx
+++ b/Documents/RPi NTP Time Server Statrum-2/Test/TestLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thaonguyen\Desktop\KLTN\Documents\RPi NTP Time Server Statrum-2\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B08A1816-ABD7-4B8B-B3C8-842F2D518DD2}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{339815F9-9FED-47D9-A077-18936CA7C33F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5652" xr2:uid="{A6CB2F83-FF15-4450-A456-F601A008AE4D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>Time</t>
   </si>
@@ -87,13 +87,22 @@
 - GPS placed near window, pps led blink
 - GPS Module connect to Rpi directly via GPIO</t>
   </si>
+  <si>
+    <t>- Without internet
+- 2 Raspberry Pi was been put outdoor for more than 8 hours (from 10pm to 6am)
+- First login after boot at 6am</t>
+  </si>
+  <si>
+    <t>- My Raspberry seem to work good with timing correct within 1ms
+- Khoa's Raspberry timing correct within 90ms</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="h:mm;@"/>
+    <numFmt numFmtId="164" formatCode="h:mm;@"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -206,12 +215,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -229,10 +232,10 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -256,6 +259,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -573,8 +582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10BC1D4B-31FD-4EF9-BDD9-CA2E665D5CAB}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5:E6"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -584,17 +593,17 @@
     <col min="3" max="3" width="25.77734375" style="1" customWidth="1"/>
     <col min="4" max="5" width="50.77734375" customWidth="1"/>
     <col min="6" max="6" width="50.77734375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="50.77734375" style="20" customWidth="1"/>
+    <col min="7" max="7" width="50.77734375" style="18" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="5"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="23"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
@@ -612,46 +621,46 @@
       <c r="E2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="21"/>
+      <c r="G2" s="19"/>
     </row>
     <row r="3" spans="1:7" ht="106.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="B3" s="13">
+      <c r="B3" s="11">
         <v>43201</v>
       </c>
-      <c r="C3" s="14">
+      <c r="C3" s="12">
         <v>0.56180555555555556</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="22"/>
+      <c r="F3" s="20"/>
     </row>
     <row r="4" spans="1:7" ht="106.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>2</v>
       </c>
-      <c r="B4" s="13">
+      <c r="B4" s="11">
         <v>43201</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C4" s="12">
         <v>0.59097222222222223</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="23" t="s">
+      <c r="F4" s="21" t="s">
         <v>10</v>
       </c>
     </row>
@@ -659,19 +668,19 @@
       <c r="A5" s="3">
         <v>3</v>
       </c>
-      <c r="B5" s="13">
+      <c r="B5" s="11">
         <v>43201</v>
       </c>
-      <c r="C5" s="14">
+      <c r="C5" s="12">
         <v>0.61527777777777781</v>
       </c>
-      <c r="D5" s="18" t="s">
+      <c r="D5" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="18" t="s">
+      <c r="E5" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="23" t="s">
+      <c r="F5" s="21" t="s">
         <v>11</v>
       </c>
     </row>
@@ -679,128 +688,136 @@
       <c r="A6" s="3">
         <v>4</v>
       </c>
-      <c r="B6" s="13">
+      <c r="B6" s="11">
         <v>43201</v>
       </c>
-      <c r="C6" s="14">
+      <c r="C6" s="12">
         <v>0.63680555555555551</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D6" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="18" t="s">
+      <c r="E6" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="22"/>
-    </row>
-    <row r="7" spans="1:7" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="F6" s="20"/>
+    </row>
+    <row r="7" spans="1:7" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>5</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="22"/>
+      <c r="B7" s="11">
+        <v>43209</v>
+      </c>
+      <c r="C7" s="12">
+        <v>0.27291666666666664</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="20"/>
     </row>
     <row r="8" spans="1:7" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>6</v>
       </c>
       <c r="B8" s="3"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="22"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="20"/>
     </row>
     <row r="9" spans="1:7" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>7</v>
       </c>
       <c r="B9" s="3"/>
-      <c r="C9" s="14"/>
-      <c r="D9" s="16"/>
-      <c r="E9" s="16"/>
-      <c r="F9" s="22"/>
+      <c r="C9" s="12"/>
+      <c r="D9" s="14"/>
+      <c r="E9" s="14"/>
+      <c r="F9" s="20"/>
     </row>
     <row r="10" spans="1:7" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>8</v>
       </c>
       <c r="B10" s="3"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="16"/>
-      <c r="E10" s="16"/>
-      <c r="F10" s="22"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="20"/>
     </row>
     <row r="11" spans="1:7" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>9</v>
       </c>
       <c r="B11" s="3"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="22"/>
+      <c r="C11" s="12"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="20"/>
     </row>
     <row r="12" spans="1:7" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="7">
+      <c r="A12" s="5">
         <v>10</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
-      <c r="F12" s="22"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="13"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="20"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="10"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
+      <c r="A13" s="8"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="8"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
+      <c r="A14" s="6"/>
+      <c r="B14" s="4"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="8"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
+      <c r="A15" s="6"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="8"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
+      <c r="A16" s="6"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="8"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
+      <c r="A17" s="6"/>
+      <c r="B17" s="4"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="8"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="9"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
+      <c r="A18" s="6"/>
+      <c r="B18" s="4"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="8"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
+      <c r="A19" s="6"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Update: Them 2 lan test dong bong thoi gian voi LoRa module
</commit_message>
<xml_diff>
--- a/Documents/RPi NTP Time Server Statrum-2/Test/TestLog.xlsx
+++ b/Documents/RPi NTP Time Server Statrum-2/Test/TestLog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thaonguyen\Desktop\KLTN\Documents\RPi NTP Time Server Statrum-2\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{339815F9-9FED-47D9-A077-18936CA7C33F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7BCD696-6A85-4A2C-B194-D84F80251E46}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5652" xr2:uid="{A6CB2F83-FF15-4450-A456-F601A008AE4D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="5655" xr2:uid="{A6CB2F83-FF15-4450-A456-F601A008AE4D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
   <si>
     <t>Time</t>
   </si>
@@ -95,6 +95,26 @@
   <si>
     <t>- My Raspberry seem to work good with timing correct within 1ms
 - Khoa's Raspberry timing correct within 90ms</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- After 10 min, black Rpi lock to gps with time correct within 1ms and red Rpi lock to gps with time correct within 4ms
+- </t>
+  </si>
+  <si>
+    <t>- With internet from laptop (laptop is connected to Ethernet)
+- Lora transmitter is connected to laptop via usb uart CP2102 and transmit 26 packages each reset time
+- Each Rpi is connected with an LoRa reciver via an USB UART at /dev/ttyUSB0 and an ublox neo 7 GPS
+- Both Rpi ntp can synchronize with each other via LAN
+- Test indoor, room E6.1, 2 GPS with next by the window
+- 2 LoRa receiver is put side by side</t>
+  </si>
+  <si>
+    <t>- With internet from laptop (laptop is connected to phone's Ethernet)
+- Lora transmitter is connected to laptop via usb uart CP2102 and transmit 26 packages each reset time
+- Each Rpi is connected with an LoRa reciver via an USB UART at /dev/ttyUSB0 and an ublox neo 7 GPS
+- Both Rpi ntp can synchronize with each other via LAN
+- Test outdoor, roof of E building
+- 2 LoRa receiver is put side by side</t>
   </si>
 </sst>
 </file>
@@ -582,21 +602,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10BC1D4B-31FD-4EF9-BDD9-CA2E665D5CAB}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.21875" customWidth="1"/>
-    <col min="2" max="2" width="25.77734375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="25.77734375" style="1" customWidth="1"/>
-    <col min="4" max="5" width="50.77734375" customWidth="1"/>
-    <col min="6" max="6" width="50.77734375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="50.77734375" style="18" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" style="1" customWidth="1"/>
+    <col min="4" max="5" width="50.7109375" customWidth="1"/>
+    <col min="6" max="6" width="50.7109375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="50.7109375" style="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
         <v>1</v>
       </c>
@@ -605,7 +625,7 @@
       <c r="D1" s="22"/>
       <c r="E1" s="23"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -626,7 +646,7 @@
       </c>
       <c r="G2" s="19"/>
     </row>
-    <row r="3" spans="1:7" ht="106.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="106.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1</v>
       </c>
@@ -644,7 +664,7 @@
       </c>
       <c r="F3" s="20"/>
     </row>
-    <row r="4" spans="1:7" ht="106.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="106.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>2</v>
       </c>
@@ -664,7 +684,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="79.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="79.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>3</v>
       </c>
@@ -684,7 +704,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>4</v>
       </c>
@@ -702,7 +722,7 @@
       </c>
       <c r="F6" s="20"/>
     </row>
-    <row r="7" spans="1:7" ht="86.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="86.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>5</v>
       </c>
@@ -720,27 +740,41 @@
       </c>
       <c r="F7" s="20"/>
     </row>
-    <row r="8" spans="1:7" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="144" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>6</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
+      <c r="B8" s="11">
+        <v>43210</v>
+      </c>
+      <c r="C8" s="12">
+        <v>0.69444444444444453</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>16</v>
+      </c>
       <c r="F8" s="20"/>
     </row>
-    <row r="9" spans="1:7" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="199.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>7</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="14"/>
+      <c r="B9" s="11">
+        <v>43210</v>
+      </c>
+      <c r="C9" s="12">
+        <v>0.71597222222222223</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>18</v>
+      </c>
       <c r="E9" s="14"/>
       <c r="F9" s="20"/>
     </row>
-    <row r="10" spans="1:7" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>8</v>
       </c>
@@ -750,7 +784,7 @@
       <c r="E10" s="14"/>
       <c r="F10" s="20"/>
     </row>
-    <row r="11" spans="1:7" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>9</v>
       </c>
@@ -760,7 +794,7 @@
       <c r="E11" s="14"/>
       <c r="F11" s="20"/>
     </row>
-    <row r="12" spans="1:7" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="5">
         <v>10</v>
       </c>
@@ -770,49 +804,49 @@
       <c r="E12" s="15"/>
       <c r="F12" s="20"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="8"/>
       <c r="B13" s="9"/>
       <c r="C13" s="10"/>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
       <c r="B14" s="4"/>
       <c r="C14" s="7"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
       <c r="B15" s="4"/>
       <c r="C15" s="7"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
       <c r="B16" s="4"/>
       <c r="C16" s="7"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
       <c r="B17" s="4"/>
       <c r="C17" s="7"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
       <c r="B18" s="4"/>
       <c r="C18" s="7"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
       <c r="B19" s="4"/>
       <c r="C19" s="7"/>

</xml_diff>

<commit_message>
Update: Them test8 RPi NTP Time Server - dong bo thoi gian qua internet, khong dung gps module
</commit_message>
<xml_diff>
--- a/Documents/RPi NTP Time Server Statrum-2/Test/TestLog.xlsx
+++ b/Documents/RPi NTP Time Server Statrum-2/Test/TestLog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thaonguyen\Desktop\KLTN\Documents\RPi NTP Time Server Statrum-2\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7BCD696-6A85-4A2C-B194-D84F80251E46}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CB4F086-0EA1-4009-8CAC-C9302BE747CD}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17250" windowHeight="5655" xr2:uid="{A6CB2F83-FF15-4450-A456-F601A008AE4D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t>Time</t>
   </si>
@@ -115,6 +115,15 @@
 - Both Rpi ntp can synchronize with each other via LAN
 - Test outdoor, roof of E building
 - 2 LoRa receiver is put side by side</t>
+  </si>
+  <si>
+    <t>- Without GPS module, time is completely synchronized from internet NTP Time server (more specific in result picture) and from each other
+- Lora transmitter is connected to laptop via usb uart CP2102 and transmit 26 packages each reset
+- Test indoor, room E6.1, 2 GPS with next by the window
+- 2 LoRa receiver is put side by side</t>
+  </si>
+  <si>
+    <t>-Result in file indoor8</t>
   </si>
 </sst>
 </file>
@@ -221,7 +230,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -285,6 +294,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -603,7 +615,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -774,14 +786,22 @@
       <c r="E9" s="14"/>
       <c r="F9" s="20"/>
     </row>
-    <row r="10" spans="1:7" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="159.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>8</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
+      <c r="B10" s="11">
+        <v>43223</v>
+      </c>
+      <c r="C10" s="12">
+        <v>0.60277777777777775</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="24" t="s">
+        <v>20</v>
+      </c>
       <c r="F10" s="20"/>
     </row>
     <row r="11" spans="1:7" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>